<commit_message>
Updated example rules file and regenerated test data for workflow test
</commit_message>
<xml_diff>
--- a/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
+++ b/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/get/neat/cognite/neat/examples/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrslivincovs/DevProject/Cognite/projects/neat/aleks-data/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6785ACA1-B455-794D-9923-DBC2F58B25A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B7DF80-1A39-6F43-8AC4-6478DD45170A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="500" windowWidth="52940" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40160" yWindow="4580" windowWidth="35560" windowHeight="19080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="152">
   <si>
     <t>shortName</t>
   </si>
@@ -774,7 +774,16 @@
     <t>sparql</t>
   </si>
   <si>
-    <t>nordic44:_2dd9048c-bdfb-11e5-94fa-c8f73332c8f4</t>
+    <t>neat:_2dd9048c-bdfb-11e5-94fa-c8f73332c8f4</t>
+  </si>
+  <si>
+    <t>neat</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat#</t>
+  </si>
+  <si>
+    <t>Neat default namespace</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1247,7 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1361,7 +1370,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1391,6 +1399,10 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -26740,8 +26752,8 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScale="207" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="207" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26869,6 +26881,17 @@
       </c>
       <c r="C11" s="65" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="81" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -26887,6 +26910,7 @@
     <hyperlink ref="B3" r:id="rId8" xr:uid="{59FA1FA9-2507-A644-B18C-514AD3518DF5}"/>
     <hyperlink ref="B4" r:id="rId9" xr:uid="{3AF693B8-84D6-C748-A981-4069BDE6B7E6}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{75538B98-5375-CF4D-B6A7-7A2A4F28FBCB}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{A5F1C332-0E06-024A-B3A4-50675E9630B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -26922,24 +26946,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="73"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -27262,7 +27286,7 @@
   </sheetPr>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -27292,34 +27316,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="76" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="75" t="s">
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="74" t="s">
+      <c r="N1" s="74"/>
+      <c r="O1" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -28149,11 +28173,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
@@ -28278,7 +28302,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="80" t="s">
         <v>148</v>
       </c>
       <c r="B13" s="42" t="s">

</xml_diff>

<commit_message>
Bug fixes in base workflows and improved data-exploration UI  (#55)
* base wf fixes and data exploration UI extensions

* more data exploration improvements


* Updated example rules file and
regenerated test data for workflow test

* updated change log and removed commented code

---------

Co-authored-by: Aleksandrs Livincovs <aleksandrs.livincovs@cognite.com>
</commit_message>
<xml_diff>
--- a/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
+++ b/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/get/neat/cognite/neat/examples/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrslivincovs/DevProject/Cognite/projects/neat/aleks-data/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6785ACA1-B455-794D-9923-DBC2F58B25A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B7DF80-1A39-6F43-8AC4-6478DD45170A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="500" windowWidth="52940" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40160" yWindow="4580" windowWidth="35560" windowHeight="19080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="152">
   <si>
     <t>shortName</t>
   </si>
@@ -774,7 +774,16 @@
     <t>sparql</t>
   </si>
   <si>
-    <t>nordic44:_2dd9048c-bdfb-11e5-94fa-c8f73332c8f4</t>
+    <t>neat:_2dd9048c-bdfb-11e5-94fa-c8f73332c8f4</t>
+  </si>
+  <si>
+    <t>neat</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat#</t>
+  </si>
+  <si>
+    <t>Neat default namespace</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1247,7 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1361,7 +1370,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1391,6 +1399,10 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -26740,8 +26752,8 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScale="207" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="207" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26869,6 +26881,17 @@
       </c>
       <c r="C11" s="65" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="81" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -26887,6 +26910,7 @@
     <hyperlink ref="B3" r:id="rId8" xr:uid="{59FA1FA9-2507-A644-B18C-514AD3518DF5}"/>
     <hyperlink ref="B4" r:id="rId9" xr:uid="{3AF693B8-84D6-C748-A981-4069BDE6B7E6}"/>
     <hyperlink ref="B11" r:id="rId10" xr:uid="{75538B98-5375-CF4D-B6A7-7A2A4F28FBCB}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{A5F1C332-0E06-024A-B3A4-50675E9630B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -26922,24 +26946,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="73"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -27262,7 +27286,7 @@
   </sheetPr>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -27292,34 +27316,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="76" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="75" t="s">
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="74" t="s">
+      <c r="N1" s="74"/>
+      <c r="O1" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -28149,11 +28173,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
@@ -28278,7 +28302,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="80" t="s">
         <v>148</v>
       </c>
       <c r="B13" s="42" t="s">

</xml_diff>

<commit_message>
updated transformation rules with namespace field in metadata
</commit_message>
<xml_diff>
--- a/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
+++ b/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrslivincovs/DevProject/Cognite/projects/neat/aleks-data/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B7DF80-1A39-6F43-8AC4-6478DD45170A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EECE7A-DDE3-7448-B7CE-2CE213421E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40160" yWindow="4580" windowWidth="35560" windowHeight="19080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33240" yWindow="4580" windowWidth="35560" windowHeight="23060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="152">
-  <si>
-    <t>shortName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="154">
   <si>
     <t>tnt</t>
   </si>
@@ -785,6 +782,15 @@
   <si>
     <t>Neat default namespace</t>
   </si>
+  <si>
+    <t>http://purl.org/cognite/tnt#</t>
+  </si>
+  <si>
+    <t>namespace</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
 </sst>
 </file>
 
@@ -1370,6 +1376,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1399,10 +1409,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1728,10 +1734,10 @@
     <tabColor rgb="FFFFE699"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W998"/>
+  <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1749,10 +1755,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1778,24 +1784,24 @@
     </row>
     <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>152</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>151</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -1805,26 +1811,26 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1834,26 +1840,26 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="9">
-        <v>44833</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -1865,10 +1871,10 @@
     </row>
     <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>44833</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
@@ -1894,10 +1900,10 @@
     </row>
     <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
@@ -1923,9 +1929,11 @@
     </row>
     <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1950,11 +1958,9 @@
     </row>
     <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1979,12 +1985,14 @@
     </row>
     <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="3"/>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
@@ -2004,18 +2012,16 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -2035,24 +2041,24 @@
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -2064,9 +2070,11 @@
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>95</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -2090,8 +2098,10 @@
       <c r="W12" s="4"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -26739,7 +26749,35 @@
       <c r="V998" s="4"/>
       <c r="W998" s="4"/>
     </row>
+    <row r="999" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A999" s="4"/>
+      <c r="B999" s="4"/>
+      <c r="C999" s="4"/>
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+      <c r="G999" s="4"/>
+      <c r="H999" s="4"/>
+      <c r="I999" s="4"/>
+      <c r="J999" s="4"/>
+      <c r="K999" s="4"/>
+      <c r="L999" s="4"/>
+      <c r="M999" s="4"/>
+      <c r="N999" s="4"/>
+      <c r="O999" s="4"/>
+      <c r="P999" s="4"/>
+      <c r="Q999" s="4"/>
+      <c r="R999" s="4"/>
+      <c r="S999" s="4"/>
+      <c r="T999" s="4"/>
+      <c r="U999" s="4"/>
+      <c r="V999" s="4"/>
+      <c r="W999" s="4"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4C5500DE-C402-7B42-8B59-6E892B1A50D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -26752,7 +26790,7 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="207" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="207" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -26764,134 +26802,134 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="C1" s="64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="60" t="s">
-        <v>53</v>
-      </c>
       <c r="C2" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="62" t="s">
-        <v>128</v>
-      </c>
       <c r="C3" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="62" t="s">
-        <v>126</v>
-      </c>
       <c r="C4" s="66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>41</v>
-      </c>
       <c r="C5" s="66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="60" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="60" t="s">
-        <v>45</v>
-      </c>
       <c r="C7" s="66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="60" t="s">
-        <v>47</v>
-      </c>
       <c r="C8" s="66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="62" t="s">
-        <v>49</v>
-      </c>
       <c r="C9" s="66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="60" t="s">
-        <v>51</v>
-      </c>
       <c r="C10" s="66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>123</v>
-      </c>
       <c r="C11" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="C12" s="66" t="s">
         <v>150</v>
-      </c>
-      <c r="C12" s="66" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -26946,76 +26984,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="72"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
+      <c r="G1" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>63</v>
-      </c>
       <c r="E2" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="12"/>
@@ -27027,17 +27065,17 @@
     </row>
     <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="12"/>
@@ -27049,15 +27087,15 @@
     </row>
     <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="12"/>
@@ -27069,13 +27107,13 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="12"/>
@@ -27087,14 +27125,14 @@
     </row>
     <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="22"/>
@@ -27107,15 +27145,15 @@
     </row>
     <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="12"/>
@@ -27127,7 +27165,7 @@
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -27316,107 +27354,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="75" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="74" t="s">
+      <c r="A1" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="76"/>
+      <c r="O1" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="74"/>
-      <c r="O1" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>67</v>
-      </c>
       <c r="G2" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="L2" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="R2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="S2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="45"/>
       <c r="D3" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="46">
         <v>1</v>
@@ -27425,20 +27463,20 @@
         <v>1</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" s="44"/>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
       <c r="M3" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N3" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
@@ -27449,14 +27487,14 @@
     </row>
     <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="45"/>
       <c r="D4" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="46">
         <v>1</v>
@@ -27465,20 +27503,20 @@
         <v>1</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="44"/>
       <c r="J4" s="44"/>
       <c r="K4" s="44"/>
       <c r="L4" s="44"/>
       <c r="M4" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N4" s="55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
@@ -27489,14 +27527,14 @@
     </row>
     <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="36">
         <v>1</v>
@@ -27505,20 +27543,20 @@
         <v>1</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
       <c r="M5" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N5" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
@@ -27529,14 +27567,14 @@
     </row>
     <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="35"/>
       <c r="D6" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="36">
         <v>1</v>
@@ -27545,20 +27583,20 @@
         <v>1</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
       <c r="M6" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N6" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
@@ -27569,14 +27607,14 @@
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="30">
         <v>1</v>
@@ -27585,20 +27623,20 @@
         <v>1</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
       <c r="M7" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N7" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
@@ -27609,14 +27647,14 @@
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="30">
         <v>1</v>
@@ -27625,20 +27663,20 @@
         <v>1</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N8" s="49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
@@ -27649,14 +27687,14 @@
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="30">
         <v>1</v>
@@ -27665,22 +27703,22 @@
         <v>1</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L9" s="28"/>
       <c r="M9" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N9" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
@@ -27691,14 +27729,14 @@
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="27">
         <v>1</v>
@@ -27707,20 +27745,20 @@
         <v>1</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
       <c r="M10" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N10" s="57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -27731,14 +27769,14 @@
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="27">
         <v>1</v>
@@ -27747,20 +27785,20 @@
         <v>1</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
       <c r="M11" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N11" s="50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -27771,14 +27809,14 @@
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="27">
         <v>1</v>
@@ -27787,22 +27825,22 @@
         <v>1</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
       <c r="K12" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N12" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
@@ -27813,16 +27851,16 @@
     </row>
     <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>30</v>
       </c>
       <c r="E13" s="21">
         <v>1</v>
@@ -27831,20 +27869,20 @@
         <v>1</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
       <c r="M13" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N13" s="58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
@@ -27855,16 +27893,16 @@
     </row>
     <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>32</v>
-      </c>
       <c r="D14" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="21">
         <v>1</v>
@@ -27873,20 +27911,20 @@
         <v>1</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
       <c r="M14" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N14" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
@@ -27897,16 +27935,16 @@
     </row>
     <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="21">
         <v>1</v>
@@ -27915,20 +27953,20 @@
         <v>1</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N15" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
@@ -27939,36 +27977,36 @@
     </row>
     <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="21">
         <v>1</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L16" s="19"/>
       <c r="M16" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N16" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
@@ -27979,14 +28017,14 @@
     </row>
     <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="32" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>28</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="33">
         <v>1</v>
@@ -27995,20 +28033,20 @@
         <v>1</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
       <c r="M17" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N17" s="54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
@@ -28019,14 +28057,14 @@
     </row>
     <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" s="33">
         <v>1</v>
@@ -28035,20 +28073,20 @@
         <v>1</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
       <c r="L18" s="32"/>
       <c r="M18" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N18" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
@@ -28059,14 +28097,14 @@
     </row>
     <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="33">
         <v>1</v>
@@ -28075,20 +28113,20 @@
         <v>1</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
       <c r="M19" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N19" s="67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
@@ -28099,14 +28137,14 @@
     </row>
     <row r="20" spans="1:20" ht="175" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="33">
         <v>1</v>
@@ -28115,22 +28153,22 @@
         <v>1</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
       <c r="K20" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L20" s="32"/>
       <c r="M20" s="69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N20" s="68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
@@ -28173,143 +28211,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="79"/>
+      <c r="A1" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="81"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>100</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>102</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="37"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="80" t="s">
-        <v>148</v>
+      <c r="A13" s="70" t="s">
+        <v>147</v>
       </c>
       <c r="B13" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revamp of TRules validations (#61)
Changed
- Parsing of Transformation Rules from Excel files more stricter validations
- Updated all notebook to work with new neat package structure

Added
- Dedicated module for exceptions (warnings/errors) for Transformation Rules parsing
- Ability to generate parsing report containing warnings/errors
- Conversion of OWL ontologies to Transformation Rules
- Notebook testing
</commit_message>
<xml_diff>
--- a/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
+++ b/cognite/neat/examples/rules/Rules-Nordic44-to-TNT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrslivincovs/DevProject/Cognite/projects/neat/aleks-data/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/examples/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B7DF80-1A39-6F43-8AC4-6478DD45170A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EECE7A-DDE3-7448-B7CE-2CE213421E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40160" yWindow="4580" windowWidth="35560" windowHeight="19080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33240" yWindow="4580" windowWidth="35560" windowHeight="23060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="152">
-  <si>
-    <t>shortName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="154">
   <si>
     <t>tnt</t>
   </si>
@@ -785,6 +782,15 @@
   <si>
     <t>Neat default namespace</t>
   </si>
+  <si>
+    <t>http://purl.org/cognite/tnt#</t>
+  </si>
+  <si>
+    <t>namespace</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
 </sst>
 </file>
 
@@ -1370,6 +1376,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1399,10 +1409,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1728,10 +1734,10 @@
     <tabColor rgb="FFFFE699"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W998"/>
+  <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1749,10 +1755,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1778,24 +1784,24 @@
     </row>
     <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>152</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>151</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -1805,26 +1811,26 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1834,26 +1840,26 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="9">
-        <v>44833</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -1865,10 +1871,10 @@
     </row>
     <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>44833</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
@@ -1894,10 +1900,10 @@
     </row>
     <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
@@ -1923,9 +1929,11 @@
     </row>
     <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1950,11 +1958,9 @@
     </row>
     <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1979,12 +1985,14 @@
     </row>
     <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="3"/>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
@@ -2004,18 +2012,16 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -2035,24 +2041,24 @@
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -2064,9 +2070,11 @@
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>95</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -2090,8 +2098,10 @@
       <c r="W12" s="4"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -26739,7 +26749,35 @@
       <c r="V998" s="4"/>
       <c r="W998" s="4"/>
     </row>
+    <row r="999" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A999" s="4"/>
+      <c r="B999" s="4"/>
+      <c r="C999" s="4"/>
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+      <c r="G999" s="4"/>
+      <c r="H999" s="4"/>
+      <c r="I999" s="4"/>
+      <c r="J999" s="4"/>
+      <c r="K999" s="4"/>
+      <c r="L999" s="4"/>
+      <c r="M999" s="4"/>
+      <c r="N999" s="4"/>
+      <c r="O999" s="4"/>
+      <c r="P999" s="4"/>
+      <c r="Q999" s="4"/>
+      <c r="R999" s="4"/>
+      <c r="S999" s="4"/>
+      <c r="T999" s="4"/>
+      <c r="U999" s="4"/>
+      <c r="V999" s="4"/>
+      <c r="W999" s="4"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4C5500DE-C402-7B42-8B59-6E892B1A50D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -26752,7 +26790,7 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="207" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="207" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -26764,134 +26802,134 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="C1" s="64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="60" t="s">
-        <v>53</v>
-      </c>
       <c r="C2" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="62" t="s">
-        <v>128</v>
-      </c>
       <c r="C3" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="62" t="s">
-        <v>126</v>
-      </c>
       <c r="C4" s="66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>41</v>
-      </c>
       <c r="C5" s="66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="60" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="60" t="s">
-        <v>45</v>
-      </c>
       <c r="C7" s="66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="60" t="s">
-        <v>47</v>
-      </c>
       <c r="C8" s="66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="62" t="s">
-        <v>49</v>
-      </c>
       <c r="C9" s="66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="60" t="s">
-        <v>51</v>
-      </c>
       <c r="C10" s="66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>123</v>
-      </c>
       <c r="C11" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="C12" s="66" t="s">
         <v>150</v>
-      </c>
-      <c r="C12" s="66" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -26946,76 +26984,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="72"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
+      <c r="G1" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>63</v>
-      </c>
       <c r="E2" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="12"/>
@@ -27027,17 +27065,17 @@
     </row>
     <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="12"/>
@@ -27049,15 +27087,15 @@
     </row>
     <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="12"/>
@@ -27069,13 +27107,13 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="12"/>
@@ -27087,14 +27125,14 @@
     </row>
     <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="22"/>
@@ -27107,15 +27145,15 @@
     </row>
     <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="12"/>
@@ -27127,7 +27165,7 @@
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -27316,107 +27354,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="75" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="74" t="s">
+      <c r="A1" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="76"/>
+      <c r="O1" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="74"/>
-      <c r="O1" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
     </row>
     <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>67</v>
-      </c>
       <c r="G2" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="L2" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="Q2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="R2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="S2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="45"/>
       <c r="D3" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="46">
         <v>1</v>
@@ -27425,20 +27463,20 @@
         <v>1</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" s="44"/>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
       <c r="M3" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N3" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
@@ -27449,14 +27487,14 @@
     </row>
     <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="45"/>
       <c r="D4" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="46">
         <v>1</v>
@@ -27465,20 +27503,20 @@
         <v>1</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="44"/>
       <c r="J4" s="44"/>
       <c r="K4" s="44"/>
       <c r="L4" s="44"/>
       <c r="M4" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N4" s="55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
@@ -27489,14 +27527,14 @@
     </row>
     <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="36">
         <v>1</v>
@@ -27505,20 +27543,20 @@
         <v>1</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
       <c r="M5" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N5" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
@@ -27529,14 +27567,14 @@
     </row>
     <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="35"/>
       <c r="D6" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="36">
         <v>1</v>
@@ -27545,20 +27583,20 @@
         <v>1</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
       <c r="M6" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N6" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
@@ -27569,14 +27607,14 @@
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="30">
         <v>1</v>
@@ -27585,20 +27623,20 @@
         <v>1</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
       <c r="M7" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N7" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
@@ -27609,14 +27647,14 @@
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="30">
         <v>1</v>
@@ -27625,20 +27663,20 @@
         <v>1</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N8" s="49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
@@ -27649,14 +27687,14 @@
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="30">
         <v>1</v>
@@ -27665,22 +27703,22 @@
         <v>1</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L9" s="28"/>
       <c r="M9" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N9" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
@@ -27691,14 +27729,14 @@
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="27">
         <v>1</v>
@@ -27707,20 +27745,20 @@
         <v>1</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
       <c r="M10" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N10" s="57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -27731,14 +27769,14 @@
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="27">
         <v>1</v>
@@ -27747,20 +27785,20 @@
         <v>1</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
       <c r="M11" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N11" s="50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -27771,14 +27809,14 @@
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="27">
         <v>1</v>
@@ -27787,22 +27825,22 @@
         <v>1</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
       <c r="K12" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N12" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
@@ -27813,16 +27851,16 @@
     </row>
     <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>30</v>
       </c>
       <c r="E13" s="21">
         <v>1</v>
@@ -27831,20 +27869,20 @@
         <v>1</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
       <c r="M13" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N13" s="58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
@@ -27855,16 +27893,16 @@
     </row>
     <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>32</v>
-      </c>
       <c r="D14" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="21">
         <v>1</v>
@@ -27873,20 +27911,20 @@
         <v>1</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
       <c r="M14" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N14" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
@@ -27897,16 +27935,16 @@
     </row>
     <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="21">
         <v>1</v>
@@ -27915,20 +27953,20 @@
         <v>1</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N15" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
@@ -27939,36 +27977,36 @@
     </row>
     <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="21">
         <v>1</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L16" s="19"/>
       <c r="M16" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N16" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
@@ -27979,14 +28017,14 @@
     </row>
     <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="32" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>28</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="33">
         <v>1</v>
@@ -27995,20 +28033,20 @@
         <v>1</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
       <c r="M17" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N17" s="54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
@@ -28019,14 +28057,14 @@
     </row>
     <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" s="33">
         <v>1</v>
@@ -28035,20 +28073,20 @@
         <v>1</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
       <c r="L18" s="32"/>
       <c r="M18" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N18" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
@@ -28059,14 +28097,14 @@
     </row>
     <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="33">
         <v>1</v>
@@ -28075,20 +28113,20 @@
         <v>1</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
       <c r="M19" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N19" s="67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
@@ -28099,14 +28137,14 @@
     </row>
     <row r="20" spans="1:20" ht="175" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="33">
         <v>1</v>
@@ -28115,22 +28153,22 @@
         <v>1</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
       <c r="K20" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L20" s="32"/>
       <c r="M20" s="69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N20" s="68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
@@ -28173,143 +28211,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="79"/>
+      <c r="A1" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="81"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>100</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>102</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="37"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="80" t="s">
-        <v>148</v>
+      <c r="A13" s="70" t="s">
+        <v>147</v>
       </c>
       <c r="B13" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>